<commit_message>
AZ Aggreate Data Update 10052020.
AZ Aggreate Data Update 10052020.  Using the true source data for AMA.
</commit_message>
<xml_diff>
--- a/Arizona/AggregatedAmounts/AZ_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/Arizona/AggregatedAmounts/AZ_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Arizona\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BCD935-3664-47B0-B853-96142781E1B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003250C0-2620-47D9-9CE1-A10BFAB31D69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="5" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="6" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="252">
   <si>
     <t>Name</t>
   </si>
@@ -677,25 +677,7 @@
     <t>AZ</t>
   </si>
   <si>
-    <t>Basin Code</t>
-  </si>
-  <si>
-    <t>Groundwater</t>
-  </si>
-  <si>
     <t>(blank)</t>
-  </si>
-  <si>
-    <t>AMA_plu counter?, or AZ_counter</t>
-  </si>
-  <si>
-    <t>Water Type</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Quantity</t>
   </si>
   <si>
     <t>Unspecified</t>
@@ -746,76 +728,79 @@
     <t>AZ_Consumptive Use</t>
   </si>
   <si>
-    <t>AZ_ + counter</t>
-  </si>
-  <si>
-    <t>AMA Name</t>
-  </si>
-  <si>
-    <t>Inflow, Outflow</t>
-  </si>
-  <si>
-    <t>Incidental Recharge
-Canal Seepage
-Cut to the Aquifer
-CAGRD Replenishment
-Groundwater Inflow
-Mountain-front Recharge
-Streambed Recharge
-Groundwater Demand
-Groundwater Outflow
-Riparian Demand</t>
-  </si>
-  <si>
     <t>From Component in source data</t>
-  </si>
-  <si>
-    <t>2) Nothing really tied to a WS right now.  Keeping it simple and using 'Unspecified' for now.</t>
-  </si>
-  <si>
-    <t>Notes pertaining to state's organization Aggregated Data.</t>
-  </si>
-  <si>
-    <t>1) Using 'Inflow' and 'Outflow' from source data for the VariableCVs for now.  Technicaly we should be using more high level like "Demand", Withdrawal", "Recharge", but this is a good temp fix.</t>
-  </si>
-  <si>
-    <t>3) We incldued the Components from source data as 'VariableSpecificCV'.</t>
-  </si>
-  <si>
-    <t>4) Some of the 'Quantity' values from source data are blank, which are used for the 'Amounts' field in WaDE.  Included '' = '0' in pre-procesing code.</t>
-  </si>
-  <si>
-    <t>5) Might be an issue with csv not being able to hold geometry field well.  Seems to only be issue when csv is openend.</t>
-  </si>
-  <si>
-    <t>Notes for local QA that need to be changed for Live</t>
-  </si>
-  <si>
-    <t>1) incldue Inflow and Outflow for AZ in CVs.Variable table.</t>
-  </si>
-  <si>
-    <t>2) included Custom for AZ into CVs.ReportingUnitType table</t>
-  </si>
-  <si>
-    <t>3) included list of terms for VariableSpecificCV (see Variables tab for for list).</t>
-  </si>
-  <si>
-    <t>4) Had to update CVs.ReportYearCV with 1985-1989</t>
   </si>
   <si>
     <t>ADWR_AMA</t>
   </si>
   <si>
-    <t>6) Left Gemoetry in ReportingUnits blank for now in python code.</t>
-  </si>
-  <si>
-    <t>5) Had to update CVs.WaterSourceType with: GSF (EFFLUENT), GSF (CAP), Remediation water, Water withdrawn from wells.</t>
-  </si>
-  <si>
     <t>Active Management Area</t>
   </si>
   <si>
-    <t>6) Had to include Active Management Area in CVs.ReportingUnitType table..</t>
+    <t>State:</t>
+  </si>
+  <si>
+    <t>Organizaitons:</t>
+  </si>
+  <si>
+    <t>Data Links:</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Airzona</t>
+  </si>
+  <si>
+    <t>Airzona Deparment of Water Resources</t>
+  </si>
+  <si>
+    <t>Use this Data: http://www.azwater.gov/querycenter/query.aspx?qrysessionid=8CF17C8B1CB88E14E0534C64850A39FA</t>
+  </si>
+  <si>
+    <t>Use this as a guide line: https://new.azwater.gov/ama/ama-data</t>
+  </si>
+  <si>
+    <t>Surface Ground Water</t>
+  </si>
+  <si>
+    <t>'Allotment
+Demand
+Incidental Recharge
+Exempt Wells
+Population
+Natural
+Supply</t>
+  </si>
+  <si>
+    <t>See Custom list derived from Parent Water Type and Budget Element</t>
+  </si>
+  <si>
+    <t>AMA</t>
+  </si>
+  <si>
+    <t>Get from ReportingUnit sheet'</t>
+  </si>
+  <si>
+    <t>Get from Variable Sheet, pass in CATEGORY</t>
+  </si>
+  <si>
+    <t>Get from Watersource Sheet, pass in custom list</t>
+  </si>
+  <si>
+    <t>Use custom amount list</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>SECTOR</t>
+  </si>
+  <si>
+    <t>AZagg_plu counter?, or AZag_WS + counter</t>
+  </si>
+  <si>
+    <t>AZag_RU + counter</t>
   </si>
 </sst>
 </file>
@@ -928,7 +913,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -950,7 +935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1169,12 +1154,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1320,9 +1314,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1459,7 +1450,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1487,9 +1477,23 @@
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1805,83 +1809,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE91C3C-F676-4E77-8227-802554E4B42D}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" style="104" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="106" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="106" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="106" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="106" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="106" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="107" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="108" t="s">
-        <v>255</v>
-      </c>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="104" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="104" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="104" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="108" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="108" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="107"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="107"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="107"/>
+      <c r="C9" s="107"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="107"/>
+      <c r="C10" s="107"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="107"/>
+      <c r="C11" s="107"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="104" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" s="107"/>
+      <c r="C13" s="107"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="105"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="104"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1894,7 +1906,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1913,10 +1925,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="80"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
+      <c r="A1" s="79"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1929,7 +1941,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="80" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1961,22 +1973,22 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="82" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="84">
+      <c r="I3" s="83">
         <v>11</v>
       </c>
       <c r="J3" s="17" t="s">
@@ -1996,19 +2008,19 @@
       <c r="D4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="85" t="s">
-        <v>227</v>
+      <c r="E4" s="84" t="s">
+        <v>221</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="85" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I4" s="83" t="s">
         <v>106</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -2025,13 +2037,13 @@
       <c r="C5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="F5" s="87" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="35" t="s">
@@ -2040,7 +2052,7 @@
       <c r="H5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="83" t="s">
         <v>108</v>
       </c>
       <c r="J5" s="17" t="s">
@@ -2060,10 +2072,10 @@
       <c r="D6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="87" t="s">
-        <v>214</v>
-      </c>
-      <c r="F6" s="87" t="s">
+      <c r="E6" s="86" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="35" t="s">
@@ -2072,7 +2084,7 @@
       <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="88">
+      <c r="I6" s="87">
         <v>0.5</v>
       </c>
       <c r="J6" s="17" t="s">
@@ -2092,10 +2104,10 @@
       <c r="D7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="87" t="s">
-        <v>214</v>
-      </c>
-      <c r="F7" s="87" t="s">
+      <c r="E7" s="86" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="35" t="s">
@@ -2104,7 +2116,7 @@
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="87" t="s">
+      <c r="I7" s="86" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="17" t="s">
@@ -2121,13 +2133,13 @@
       <c r="C8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="87" t="s">
-        <v>214</v>
-      </c>
-      <c r="F8" s="87" t="s">
+      <c r="E8" s="86" t="s">
+        <v>212</v>
+      </c>
+      <c r="F8" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="35" t="s">
@@ -2136,7 +2148,7 @@
       <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="87" t="s">
+      <c r="I8" s="86" t="s">
         <v>115</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -2157,9 +2169,9 @@
         <v>11</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="F9" s="87" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="35" t="s">
@@ -2187,9 +2199,9 @@
         <v>11</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="F10" s="87" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="35" t="s">
@@ -2198,7 +2210,7 @@
       <c r="H10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="84" t="s">
+      <c r="I10" s="83" t="s">
         <v>121</v>
       </c>
       <c r="J10" s="17" t="s">
@@ -2218,10 +2230,10 @@
       <c r="D11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="103" t="s">
-        <v>228</v>
-      </c>
-      <c r="F11" s="87" t="s">
+      <c r="E11" s="101" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="35" t="s">
@@ -2230,7 +2242,7 @@
       <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="83" t="s">
         <v>124</v>
       </c>
       <c r="J11" s="17" t="s">
@@ -2247,13 +2259,13 @@
       <c r="C12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="87" t="s">
+      <c r="F12" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="35" t="s">
@@ -2262,7 +2274,7 @@
       <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="84" t="s">
+      <c r="I12" s="83" t="s">
         <v>127</v>
       </c>
       <c r="J12" s="17" t="s">
@@ -2285,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5623B452-6320-41F9-A4C3-771E435FA050}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2321,7 +2333,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="80" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -2353,16 +2365,16 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="89"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="88"/>
       <c r="H3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="84">
+      <c r="I3" s="83">
         <v>16</v>
       </c>
       <c r="J3" s="17" t="s">
@@ -2383,14 +2395,14 @@
         <v>11</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="34"/>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I4" s="83" t="s">
         <v>129</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -2414,11 +2426,11 @@
         <v>1</v>
       </c>
       <c r="F5" s="26"/>
-      <c r="G5" s="98"/>
+      <c r="G5" s="96"/>
       <c r="H5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="84">
+      <c r="I5" s="83">
         <v>1</v>
       </c>
       <c r="J5" s="17" t="s">
@@ -2435,18 +2447,18 @@
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>134</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="98"/>
+      <c r="G6" s="96"/>
       <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="84" t="s">
+      <c r="I6" s="83" t="s">
         <v>134</v>
       </c>
       <c r="J6" s="17" t="s">
@@ -2463,18 +2475,18 @@
       <c r="C7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F7" s="26"/>
-      <c r="G7" s="98"/>
+      <c r="G7" s="96"/>
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="83" t="s">
         <v>137</v>
       </c>
       <c r="J7" s="17" t="s">
@@ -2491,18 +2503,18 @@
       <c r="C8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>140</v>
       </c>
       <c r="F8" s="26"/>
-      <c r="G8" s="98"/>
+      <c r="G8" s="96"/>
       <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="84" t="s">
+      <c r="I8" s="83" t="s">
         <v>140</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -2519,18 +2531,18 @@
       <c r="C9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>143</v>
       </c>
       <c r="F9" s="26"/>
-      <c r="G9" s="98"/>
+      <c r="G9" s="96"/>
       <c r="H9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="84" t="s">
+      <c r="I9" s="83" t="s">
         <v>143</v>
       </c>
       <c r="J9" s="17" t="s">
@@ -2550,15 +2562,15 @@
       <c r="D10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="105" t="s">
-        <v>232</v>
+      <c r="E10" s="103" t="s">
+        <v>226</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="98"/>
+      <c r="G10" s="96"/>
       <c r="H10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="84">
+      <c r="I10" s="83">
         <v>10</v>
       </c>
       <c r="J10" s="17" t="s">
@@ -2575,18 +2587,18 @@
       <c r="C11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F11" s="26"/>
-      <c r="G11" s="98"/>
+      <c r="G11" s="96"/>
       <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="83" t="s">
         <v>149</v>
       </c>
       <c r="J11" s="17" t="s">
@@ -2603,25 +2615,25 @@
       <c r="C12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="98"/>
+      <c r="G12" s="96"/>
       <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="84" t="s">
+      <c r="I12" s="83" t="s">
         <v>152</v>
       </c>
       <c r="J12" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>154</v>
       </c>
@@ -2631,22 +2643,22 @@
       <c r="C13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="98" t="s">
-        <v>239</v>
+      <c r="G13" s="96" t="s">
+        <v>229</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="84" t="s">
+      <c r="I13" s="83" t="s">
         <v>155</v>
       </c>
       <c r="J13" s="17" t="s">
@@ -2667,7 +2679,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2702,7 +2714,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="80" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -2734,16 +2746,16 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="90" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="24" t="s">
@@ -2770,10 +2782,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="F4" s="33"/>
-      <c r="G4" s="86"/>
+      <c r="G4" s="85"/>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
@@ -2797,10 +2809,10 @@
       <c r="D5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="97" t="s">
-        <v>224</v>
-      </c>
-      <c r="F5" s="87"/>
+      <c r="E5" s="95" t="s">
+        <v>218</v>
+      </c>
+      <c r="F5" s="86"/>
       <c r="G5" s="35"/>
       <c r="H5" s="24" t="s">
         <v>11</v>
@@ -2825,10 +2837,10 @@
       <c r="D6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="97" t="s">
-        <v>223</v>
-      </c>
-      <c r="F6" s="87"/>
+      <c r="E6" s="95" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" s="86"/>
       <c r="G6" s="35"/>
       <c r="H6" s="24" t="s">
         <v>11</v>
@@ -2853,10 +2865,10 @@
       <c r="D7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="97" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" s="87"/>
+      <c r="E7" s="95" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="86"/>
       <c r="G7" s="35"/>
       <c r="H7" s="24" t="s">
         <v>11</v>
@@ -2882,9 +2894,9 @@
         <v>11</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="F8" s="87"/>
+        <v>219</v>
+      </c>
+      <c r="F8" s="86"/>
       <c r="G8" s="35"/>
       <c r="H8" s="24" t="s">
         <v>11</v>
@@ -2909,10 +2921,10 @@
       <c r="D9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="F9" s="87"/>
+      <c r="E9" s="95" t="s">
+        <v>220</v>
+      </c>
+      <c r="F9" s="86"/>
       <c r="G9" s="35"/>
       <c r="H9" s="24" t="s">
         <v>11</v>
@@ -2937,10 +2949,10 @@
       <c r="D10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="97" t="s">
-        <v>221</v>
-      </c>
-      <c r="F10" s="87"/>
+      <c r="E10" s="95" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="86"/>
       <c r="G10" s="35"/>
       <c r="H10" s="24" t="s">
         <v>11</v>
@@ -2965,10 +2977,10 @@
       <c r="D11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="97" t="s">
-        <v>222</v>
-      </c>
-      <c r="F11" s="87"/>
+      <c r="E11" s="95" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" s="86"/>
       <c r="G11" s="35"/>
       <c r="H11" s="24" t="s">
         <v>11</v>
@@ -2996,7 +3008,7 @@
       <c r="E12" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="F12" s="87"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="35"/>
       <c r="H12" s="24" t="s">
         <v>11</v>
@@ -3046,7 +3058,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3113,22 +3125,22 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="95" t="s">
+      <c r="H3" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="84">
+      <c r="I3" s="83">
         <v>34658</v>
       </c>
       <c r="J3" s="17" t="s">
@@ -3149,18 +3161,18 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="95" t="s">
+      <c r="H4" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I4" s="83" t="s">
         <v>182</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -3181,18 +3193,18 @@
         <v>11</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="87" t="s">
+        <v>212</v>
+      </c>
+      <c r="F5" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="95" t="s">
+      <c r="H5" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="I5" s="86" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="17" t="s">
@@ -3213,18 +3225,18 @@
         <v>15</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="87" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="H6" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="87" t="s">
+      <c r="I6" s="86" t="s">
         <v>11</v>
       </c>
       <c r="J6" s="17" t="s">
@@ -3241,22 +3253,22 @@
       <c r="C7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="86" t="s">
         <v>187</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="95" t="s">
+      <c r="H7" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="83" t="s">
         <v>187</v>
       </c>
       <c r="J7" s="17" t="s">
@@ -3277,18 +3289,18 @@
         <v>11</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="F8" s="87" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="84" t="s">
+      <c r="I8" s="83" t="s">
         <v>190</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -3308,26 +3320,26 @@
       <c r="D9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="87" t="s">
-        <v>219</v>
-      </c>
-      <c r="F9" s="87" t="s">
+      <c r="E9" s="86" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" s="86" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="95" t="s">
+      <c r="H9" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="84">
+      <c r="I9" s="83">
         <v>17839</v>
       </c>
       <c r="J9" s="17" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>194</v>
       </c>
@@ -3341,18 +3353,18 @@
         <v>15</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>11</v>
+        <v>242</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="98" t="s">
-        <v>216</v>
-      </c>
-      <c r="H10" s="95" t="s">
+      <c r="G10" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="84" t="s">
+      <c r="H10" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="83" t="s">
         <v>108</v>
       </c>
       <c r="J10" s="17" t="s">
@@ -3383,8 +3395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E3782C-18A9-45D3-B018-D5B7F7291E9F}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3445,13 +3457,13 @@
       <c r="A3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="62" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="19" t="s">
@@ -3463,13 +3475,13 @@
       <c r="G3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="95" t="s">
+      <c r="H3" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="J3" s="71" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3487,14 +3499,14 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="95" t="s">
+      <c r="H4" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="73" t="s">
         <v>97</v>
       </c>
       <c r="J4" s="41" t="s">
@@ -3514,19 +3526,19 @@
         <v>29</v>
       </c>
       <c r="D5" s="18"/>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="99" t="s">
+      <c r="F5" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="102" t="s">
+      <c r="G5" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="95" t="s">
+      <c r="H5" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="74" t="s">
         <v>102</v>
       </c>
       <c r="J5" s="40" t="s">
@@ -3546,19 +3558,19 @@
         <v>29</v>
       </c>
       <c r="D6" s="18"/>
-      <c r="E6" s="99" t="s">
+      <c r="E6" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="99" t="s">
+      <c r="F6" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="102" t="s">
+      <c r="G6" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="H6" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="77" t="s">
+      <c r="I6" s="76" t="s">
         <v>103</v>
       </c>
       <c r="J6" s="40" t="s">
@@ -3578,19 +3590,19 @@
         <v>11</v>
       </c>
       <c r="D7" s="18"/>
-      <c r="E7" s="99" t="s">
+      <c r="E7" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="99" t="s">
+      <c r="F7" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="100" t="s">
-        <v>236</v>
-      </c>
-      <c r="H7" s="95" t="s">
+      <c r="G7" s="98" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="73" t="s">
+      <c r="I7" s="72" t="s">
         <v>98</v>
       </c>
       <c r="J7" s="40" t="s">
@@ -3610,19 +3622,19 @@
         <v>11</v>
       </c>
       <c r="D8" s="18"/>
-      <c r="E8" s="101" t="s">
+      <c r="E8" s="99" t="s">
+        <v>212</v>
+      </c>
+      <c r="F8" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="99" t="s">
+      <c r="G8" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="102" t="s">
-        <v>212</v>
-      </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="73">
+      <c r="I8" s="72">
         <v>48001</v>
       </c>
       <c r="J8" s="44" t="s">
@@ -3642,19 +3654,19 @@
         <v>29</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="99" t="s">
+      <c r="E9" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="99" t="s">
+      <c r="F9" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="102" t="s">
+      <c r="G9" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="95" t="s">
+      <c r="H9" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="95" t="s">
+      <c r="I9" s="94" t="s">
         <v>11</v>
       </c>
       <c r="J9" s="40" t="s">
@@ -3674,19 +3686,19 @@
         <v>11</v>
       </c>
       <c r="D10" s="18"/>
-      <c r="E10" s="99" t="s">
-        <v>254</v>
-      </c>
-      <c r="F10" s="99" t="s">
+      <c r="E10" s="97" t="s">
+        <v>231</v>
+      </c>
+      <c r="F10" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="102" t="s">
+      <c r="G10" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="95" t="s">
+      <c r="H10" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="72" t="s">
         <v>99</v>
       </c>
       <c r="J10" s="44" t="s">
@@ -3706,19 +3718,19 @@
         <v>29</v>
       </c>
       <c r="D11" s="18"/>
-      <c r="E11" s="99" t="s">
+      <c r="E11" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="99" t="s">
+      <c r="F11" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="102" t="s">
+      <c r="G11" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="95" t="s">
+      <c r="H11" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="76" t="s">
+      <c r="I11" s="75" t="s">
         <v>100</v>
       </c>
       <c r="J11" s="44" t="s">
@@ -3738,19 +3750,19 @@
         <v>11</v>
       </c>
       <c r="D12" s="18"/>
-      <c r="E12" s="99" t="s">
+      <c r="E12" s="97" t="s">
         <v>211</v>
       </c>
-      <c r="F12" s="99" t="s">
+      <c r="F12" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="102" t="s">
+      <c r="G12" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="95" t="s">
+      <c r="H12" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="72" t="s">
         <v>101</v>
       </c>
       <c r="J12" s="40" t="s">
@@ -3855,8 +3867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E07544-54C6-4298-B1F4-AA27E9BE2694}">
   <dimension ref="A1:K16431"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3875,32 +3887,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="A1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="57" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -3914,16 +3926,16 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="61" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="14"/>
@@ -3935,21 +3947,21 @@
       <c r="I3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="50" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="62" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="19"/>
@@ -3961,21 +3973,21 @@
       <c r="I4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="50" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="62" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="19"/>
@@ -3987,21 +3999,21 @@
       <c r="I5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="50" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="62" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="19"/>
@@ -4013,21 +4025,21 @@
       <c r="I6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="50" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="62" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="19"/>
@@ -4039,21 +4051,21 @@
       <c r="I7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="62" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="19"/>
@@ -4065,24 +4077,26 @@
       <c r="I8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="51" t="s">
+      <c r="J8" s="50" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="49"/>
+      <c r="E9" s="110" t="s">
+        <v>221</v>
+      </c>
       <c r="F9" s="42"/>
       <c r="G9" s="39"/>
       <c r="H9" s="16" t="s">
@@ -4097,20 +4111,20 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>251</v>
+      <c r="E10" s="109" t="s">
+        <v>230</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="22"/>
@@ -4126,19 +4140,21 @@
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="26"/>
+      <c r="E11" s="26" t="s">
+        <v>244</v>
+      </c>
       <c r="G11" s="39"/>
       <c r="H11" s="16" t="s">
         <v>11</v>
@@ -4151,19 +4167,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="26" t="s">
+        <v>245</v>
+      </c>
       <c r="F12" s="36"/>
       <c r="G12" s="39"/>
       <c r="H12" s="16" t="s">
@@ -4178,19 +4196,21 @@
       <c r="K12" s="36"/>
     </row>
     <row r="13" spans="1:11" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="47"/>
+      <c r="E13" s="47" t="s">
+        <v>246</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="48"/>
       <c r="H13" s="16" t="s">
@@ -4217,7 +4237,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>11</v>
@@ -4231,7 +4251,7 @@
       <c r="I14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="51"/>
+      <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4247,13 +4267,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="50" t="s">
-        <v>218</v>
+      <c r="G15" s="49" t="s">
+        <v>248</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>11</v>
@@ -4261,7 +4281,7 @@
       <c r="I15" s="27">
         <v>125483.1563</v>
       </c>
-      <c r="J15" s="51" t="s">
+      <c r="J15" s="50" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4284,14 +4304,14 @@
       <c r="F16" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="50" t="s">
-        <v>217</v>
+      <c r="G16" s="25" t="s">
+        <v>249</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="J16" s="51" t="s">
+      <c r="J16" s="50" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4309,7 +4329,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>11</v>
@@ -4323,7 +4343,7 @@
       <c r="I17" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="51" t="s">
+      <c r="J17" s="50" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4337,11 +4357,11 @@
       <c r="C18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>11</v>
@@ -4355,7 +4375,7 @@
       <c r="I18" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="51" t="s">
+      <c r="J18" s="50" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4369,11 +4389,11 @@
       <c r="C19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>11</v>
@@ -4387,7 +4407,7 @@
       <c r="I19" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J19" s="51" t="s">
+      <c r="J19" s="50" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4401,11 +4421,11 @@
       <c r="C20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="104">
-        <v>43997</v>
+      <c r="E20" s="102">
+        <v>44106</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>11</v>
@@ -4419,7 +4439,7 @@
       <c r="I20" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="J20" s="51" t="s">
+      <c r="J20" s="50" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4433,11 +4453,11 @@
       <c r="C21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="D21" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>11</v>
@@ -4451,7 +4471,7 @@
       <c r="I21" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="51" t="s">
+      <c r="J21" s="50" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4469,7 +4489,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>11</v>
@@ -4483,7 +4503,7 @@
       <c r="I22" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="51" t="s">
+      <c r="J22" s="50" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4501,7 +4521,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F23" s="24" t="s">
         <v>11</v>
@@ -4515,7 +4535,7 @@
       <c r="I23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="51" t="s">
+      <c r="J23" s="50" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4533,7 +4553,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>11</v>
@@ -4547,7 +4567,7 @@
       <c r="I24" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="51" t="s">
+      <c r="J24" s="50" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4561,11 +4581,11 @@
       <c r="C25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>11</v>
@@ -4579,7 +4599,7 @@
       <c r="I25" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="51" t="s">
+      <c r="J25" s="50" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4597,7 +4617,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>11</v>
@@ -4611,7 +4631,7 @@
       <c r="I26" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="51" t="s">
+      <c r="J26" s="50" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4629,7 +4649,7 @@
         <v>11</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>11</v>
@@ -4643,7 +4663,7 @@
       <c r="I27" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="51" t="s">
+      <c r="J27" s="50" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4657,11 +4677,11 @@
       <c r="C28" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>11</v>
@@ -4675,7 +4695,7 @@
       <c r="I28" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J28" s="51"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -4687,11 +4707,11 @@
       <c r="C29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="50" t="s">
+      <c r="D29" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F29" s="24" t="s">
         <v>11</v>
@@ -4705,7 +4725,7 @@
       <c r="I29" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="J29" s="51" t="s">
+      <c r="J29" s="50" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4719,7 +4739,7 @@
       <c r="C30" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="24" t="s">
@@ -4728,7 +4748,7 @@
       <c r="F30" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="25" t="s">
         <v>134</v>
       </c>
       <c r="H30" s="16" t="s">
@@ -4737,7 +4757,7 @@
       <c r="I30" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="J30" s="51" t="s">
+      <c r="J30" s="50" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4751,11 +4771,11 @@
       <c r="C31" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="50" t="s">
+      <c r="D31" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>11</v>
@@ -4769,7 +4789,7 @@
       <c r="I31" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J31" s="51" t="s">
+      <c r="J31" s="50" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4783,11 +4803,11 @@
       <c r="C32" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="50" t="s">
+      <c r="D32" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F32" s="24" t="s">
         <v>11</v>
@@ -4801,7 +4821,7 @@
       <c r="I32" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="J32" s="51" t="s">
+      <c r="J32" s="50" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4815,11 +4835,11 @@
       <c r="C33" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="50" t="s">
+      <c r="D33" s="49" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>11</v>
@@ -4833,25 +4853,25 @@
       <c r="I33" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="J33" s="51" t="s">
+      <c r="J33" s="50" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I34" s="27"/>
-      <c r="J34" s="51"/>
+      <c r="J34" s="50"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I35" s="27"/>
-      <c r="J35" s="51"/>
+      <c r="J35" s="50"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I36" s="27"/>
-      <c r="J36" s="51"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I37" s="27"/>
-      <c r="J37" s="51"/>
+      <c r="J37" s="50"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I38" s="27"/>

</xml_diff>

<commit_message>
AZ Aggreated Data Update 10282020
AZ Aggreated Data Update 10282020.  Changes to VariableCV.  Includes ReadMe.
</commit_message>
<xml_diff>
--- a/Arizona/AggregatedAmounts/AZ_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/Arizona/AggregatedAmounts/AZ_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Arizona\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003250C0-2620-47D9-9CE1-A10BFAB31D69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2804285E-66F2-4677-A654-85DC5AE0444E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="6" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="2" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="253">
   <si>
     <t>Name</t>
   </si>
@@ -725,12 +725,6 @@
     <t>CalendarYear</t>
   </si>
   <si>
-    <t>AZ_Consumptive Use</t>
-  </si>
-  <si>
-    <t>From Component in source data</t>
-  </si>
-  <si>
     <t>ADWR_AMA</t>
   </si>
   <si>
@@ -764,18 +758,6 @@
     <t>Surface Ground Water</t>
   </si>
   <si>
-    <t>'Allotment
-Demand
-Incidental Recharge
-Exempt Wells
-Population
-Natural
-Supply</t>
-  </si>
-  <si>
-    <t>See Custom list derived from Parent Water Type and Budget Element</t>
-  </si>
-  <si>
     <t>AMA</t>
   </si>
   <si>
@@ -797,10 +779,25 @@
     <t>SECTOR</t>
   </si>
   <si>
-    <t>AZagg_plu counter?, or AZag_WS + counter</t>
+    <t>AZag_RU + counter</t>
   </si>
   <si>
-    <t>AZag_RU + counter</t>
+    <t>AZag_WS + counter</t>
+  </si>
+  <si>
+    <t>Only using Demand and Supply from the CATOGORY field, may come back and use other entries at a later day.</t>
+  </si>
+  <si>
+    <t>Demand, Supply</t>
+  </si>
+  <si>
+    <t>Used 'AMA WaterSourceType Dictionary.xlsx' from ADWR to build water source type.  See pre-processing code.</t>
+  </si>
+  <si>
+    <t>See provdied dictionary from ADWR.</t>
+  </si>
+  <si>
+    <t>AZ_Demand, AZ_Supply</t>
   </si>
 </sst>
 </file>
@@ -1812,7 +1809,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1825,31 +1822,31 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="104" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="104" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="104" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B6" s="108" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="108" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C7" s="107"/>
     </row>
@@ -1874,10 +1871,17 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="104" t="s">
-        <v>235</v>
-      </c>
-      <c r="B13" s="107"/>
+        <v>233</v>
+      </c>
+      <c r="B13" s="107" t="s">
+        <v>248</v>
+      </c>
       <c r="C13" s="107"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="105"/>
@@ -2041,7 +2045,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F5" s="86" t="s">
         <v>11</v>
@@ -2297,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5623B452-6320-41F9-A4C3-771E435FA050}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,7 +2399,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="34"/>
@@ -2619,7 +2623,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="96"/>
@@ -2633,7 +2637,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>154</v>
       </c>
@@ -2646,15 +2650,11 @@
       <c r="D13" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="96" t="s">
-        <v>229</v>
-      </c>
+      <c r="E13" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="96"/>
       <c r="H13" s="24" t="s">
         <v>11</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="85"/>
@@ -3058,7 +3058,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3147,7 +3147,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -3339,7 +3339,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>194</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>11</v>
@@ -3499,7 +3499,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
@@ -3597,7 +3597,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="98" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="H7" s="94" t="s">
         <v>11</v>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="97" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F10" s="97" t="s">
         <v>11</v>
@@ -3867,8 +3867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E07544-54C6-4298-B1F4-AA27E9BE2694}">
   <dimension ref="A1:K16431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4124,7 +4124,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="109" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="22"/>
@@ -4153,7 +4153,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G11" s="39"/>
       <c r="H11" s="16" t="s">
@@ -4180,7 +4180,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="39"/>
@@ -4209,7 +4209,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="47" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="48"/>
@@ -4267,13 +4267,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="49" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>11</v>
@@ -4305,7 +4305,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="27" t="s">

</xml_diff>

<commit_message>
Arizona agg data update.
Arizona agg data update.  Changes to water source.
</commit_message>
<xml_diff>
--- a/Arizona/AggregatedAmounts/AZ_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/Arizona/AggregatedAmounts/AZ_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Arizona\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2804285E-66F2-4677-A654-85DC5AE0444E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6886481-3A15-4E90-9A49-D0DCC173EB5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="2" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="645" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="WaterSources" sheetId="9" r:id="rId5"/>
     <sheet name="ReportingUnits" sheetId="4" r:id="rId6"/>
     <sheet name="AggregatedAmounts" sheetId="5" r:id="rId7"/>
+    <sheet name="watersource Dictionary" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="330">
   <si>
     <t>Name</t>
   </si>
@@ -770,9 +771,6 @@
     <t>Get from Watersource Sheet, pass in custom list</t>
   </si>
   <si>
-    <t>Use custom amount list</t>
-  </si>
-  <si>
     <t>QUANTITY</t>
   </si>
   <si>
@@ -799,6 +797,240 @@
   <si>
     <t>AZ_Demand, AZ_Supply</t>
   </si>
+  <si>
+    <t>BUDGET ELEMENT</t>
+  </si>
+  <si>
+    <t>Groundwater Allotment</t>
+  </si>
+  <si>
+    <t>Agricultural Lost and Unaccounted</t>
+  </si>
+  <si>
+    <t>Buckeye Waterlogged Area IGFRs</t>
+  </si>
+  <si>
+    <t>Exempt IGFRs</t>
+  </si>
+  <si>
+    <t>Non-Exempt IGFRs</t>
+  </si>
+  <si>
+    <t>Incidental Recharge Lagged</t>
+  </si>
+  <si>
+    <t>Incidental Recharge Total</t>
+  </si>
+  <si>
+    <t>Effluent</t>
+  </si>
+  <si>
+    <t>Groundwater</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Spill</t>
+  </si>
+  <si>
+    <t>Agricultural</t>
+  </si>
+  <si>
+    <t>Municipal</t>
+  </si>
+  <si>
+    <t>Incidental Recharge</t>
+  </si>
+  <si>
+    <t>Cattle Feedlots</t>
+  </si>
+  <si>
+    <t>Dairy Facilities</t>
+  </si>
+  <si>
+    <t>Drainage and Dewatering Permits</t>
+  </si>
+  <si>
+    <t>Non Facility Use</t>
+  </si>
+  <si>
+    <t>Power Generation Facilities</t>
+  </si>
+  <si>
+    <t>Sand and Gravel Facilities</t>
+  </si>
+  <si>
+    <t>Total Turf Demand</t>
+  </si>
+  <si>
+    <t>Domestic Exempt Volume</t>
+  </si>
+  <si>
+    <t>Large Provider Lost and Unaccounted for Water</t>
+  </si>
+  <si>
+    <t>Large Provider Non-Residential Deliveries</t>
+  </si>
+  <si>
+    <t>Large Provider Residential Deliveries</t>
+  </si>
+  <si>
+    <t>Small Provider Deliveries</t>
+  </si>
+  <si>
+    <t>Urban Irrigation</t>
+  </si>
+  <si>
+    <t>AMA Exempt Wells</t>
+  </si>
+  <si>
+    <t>AMA Exempt Well Population</t>
+  </si>
+  <si>
+    <t>Indian Reservation Population</t>
+  </si>
+  <si>
+    <t>Large Municipal Provider Population</t>
+  </si>
+  <si>
+    <t>Small Municipal Provider Population</t>
+  </si>
+  <si>
+    <t>Canal Seepage</t>
+  </si>
+  <si>
+    <t>Groundwater Inflow</t>
+  </si>
+  <si>
+    <t>Groundwater Outflow</t>
+  </si>
+  <si>
+    <t>Mountain Front</t>
+  </si>
+  <si>
+    <t>Riparian Transpiration GW</t>
+  </si>
+  <si>
+    <t>Streambed Actual</t>
+  </si>
+  <si>
+    <t>Streambed Ephemeral Actual</t>
+  </si>
+  <si>
+    <t>Streambed Ephemeral Average</t>
+  </si>
+  <si>
+    <t>Streambed Intermittent Actual</t>
+  </si>
+  <si>
+    <t>Streambed Intermittent Average</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>Poor Quality GW</t>
+  </si>
+  <si>
+    <t>Irrigation District Add ons</t>
+  </si>
+  <si>
+    <t>Direct Use Effluent</t>
+  </si>
+  <si>
+    <t>Golf Courses</t>
+  </si>
+  <si>
+    <t>Parks Schools Cemeteries HOAs</t>
+  </si>
+  <si>
+    <t>Reclaimed Water Discharge 91st 23rd</t>
+  </si>
+  <si>
+    <t>GSF (EFFLUENT)</t>
+  </si>
+  <si>
+    <t>GSF (CAP)</t>
+  </si>
+  <si>
+    <t>Deliveries to Individual Users</t>
+  </si>
+  <si>
+    <t>Excess</t>
+  </si>
+  <si>
+    <t>Recovered CAP</t>
+  </si>
+  <si>
+    <t>Recovered Effluent</t>
+  </si>
+  <si>
+    <t>Groundwater Allowance Pumping</t>
+  </si>
+  <si>
+    <t>Recovered Surface Water</t>
+  </si>
+  <si>
+    <t>Weighted Exchange Effluent</t>
+  </si>
+  <si>
+    <t>Remediation water</t>
+  </si>
+  <si>
+    <t>Mining Facilities</t>
+  </si>
+  <si>
+    <t>Recovered Reclaimed</t>
+  </si>
+  <si>
+    <t>CAP GSF</t>
+  </si>
+  <si>
+    <t>Indian Agricultural Lost and Unaccounted for water</t>
+  </si>
+  <si>
+    <t>Exception Users</t>
+  </si>
+  <si>
+    <t>Total Large Provider Demand</t>
+  </si>
+  <si>
+    <t>Net Natural Recharge In</t>
+  </si>
+  <si>
+    <t>Water withdrawn from wells</t>
+  </si>
+  <si>
+    <t>Effluent Discharge</t>
+  </si>
+  <si>
+    <t>Mexican Effluent</t>
+  </si>
+  <si>
+    <t>US Effluent</t>
+  </si>
+  <si>
+    <t>Non Conservation and Non Municipal Demand</t>
+  </si>
+  <si>
+    <t>Industrial</t>
+  </si>
+  <si>
+    <t>*Use Custom WaDE ID</t>
+  </si>
+  <si>
+    <t>*Use custom WaDE ID</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>01/01 + YEAR</t>
+  </si>
+  <si>
+    <t>12/31 + YEAR</t>
+  </si>
 </sst>
 </file>
 
@@ -807,7 +1039,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,6 +1145,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1165,7 +1404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1281,9 +1520,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1306,9 +1542,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1453,23 +1686,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1490,6 +1708,33 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1808,20 +2053,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE91C3C-F676-4E77-8227-802554E4B42D}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="104" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="97" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="97" t="s">
         <v>230</v>
       </c>
       <c r="B1" t="s">
@@ -1829,7 +2074,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="97" t="s">
         <v>231</v>
       </c>
       <c r="B2" t="s">
@@ -1837,67 +2082,67 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="101" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="101" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="107"/>
+      <c r="C7" s="100"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C8" s="107"/>
+      <c r="C8" s="100"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="100"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="107"/>
-      <c r="C11" s="107"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="100"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="107"/>
-      <c r="C12" s="107"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="97" t="s">
         <v>233</v>
       </c>
-      <c r="B13" s="107" t="s">
-        <v>248</v>
-      </c>
-      <c r="C13" s="107"/>
+      <c r="B13" s="100" t="s">
+        <v>247</v>
+      </c>
+      <c r="C13" s="100"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="105"/>
-      <c r="C20" s="106"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="99"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106"/>
-      <c r="G20" s="106"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="104"/>
-      <c r="C21" s="106"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="99"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1910,7 +2155,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1929,10 +2174,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="79"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
+      <c r="A1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1945,7 +2190,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="78" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1977,22 +2222,22 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="80" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="83">
+      <c r="I3" s="81">
         <v>11</v>
       </c>
       <c r="J3" s="17" t="s">
@@ -2012,19 +2257,19 @@
       <c r="D4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="84" t="s">
+      <c r="E4" s="82" t="s">
         <v>221</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="83" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="81" t="s">
         <v>106</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -2041,13 +2286,13 @@
       <c r="C5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="35" t="s">
@@ -2056,7 +2301,7 @@
       <c r="H5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="83" t="s">
+      <c r="I5" s="81" t="s">
         <v>108</v>
       </c>
       <c r="J5" s="17" t="s">
@@ -2076,10 +2321,10 @@
       <c r="D6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="35" t="s">
@@ -2088,7 +2333,7 @@
       <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="87">
+      <c r="I6" s="85">
         <v>0.5</v>
       </c>
       <c r="J6" s="17" t="s">
@@ -2108,10 +2353,10 @@
       <c r="D7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="86" t="s">
+      <c r="E7" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F7" s="86" t="s">
+      <c r="F7" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="35" t="s">
@@ -2120,7 +2365,7 @@
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="86" t="s">
+      <c r="I7" s="84" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="17" t="s">
@@ -2137,13 +2382,13 @@
       <c r="C8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E8" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="35" t="s">
@@ -2152,7 +2397,7 @@
       <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="86" t="s">
+      <c r="I8" s="84" t="s">
         <v>115</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -2175,7 +2420,7 @@
       <c r="E9" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="F9" s="86" t="s">
+      <c r="F9" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="35" t="s">
@@ -2205,7 +2450,7 @@
       <c r="E10" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="F10" s="86" t="s">
+      <c r="F10" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="35" t="s">
@@ -2214,7 +2459,7 @@
       <c r="H10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="83" t="s">
+      <c r="I10" s="81" t="s">
         <v>121</v>
       </c>
       <c r="J10" s="17" t="s">
@@ -2234,10 +2479,10 @@
       <c r="D11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="95" t="s">
         <v>222</v>
       </c>
-      <c r="F11" s="86" t="s">
+      <c r="F11" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="35" t="s">
@@ -2246,7 +2491,7 @@
       <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="83" t="s">
+      <c r="I11" s="81" t="s">
         <v>124</v>
       </c>
       <c r="J11" s="17" t="s">
@@ -2263,13 +2508,13 @@
       <c r="C12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="83" t="s">
+      <c r="E12" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="86" t="s">
+      <c r="F12" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="35" t="s">
@@ -2278,7 +2523,7 @@
       <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="83" t="s">
+      <c r="I12" s="81" t="s">
         <v>127</v>
       </c>
       <c r="J12" s="17" t="s">
@@ -2301,8 +2546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5623B452-6320-41F9-A4C3-771E435FA050}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2337,7 +2582,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="78" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -2369,16 +2614,16 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="88"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="86"/>
       <c r="H3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="83">
+      <c r="I3" s="81">
         <v>16</v>
       </c>
       <c r="J3" s="17" t="s">
@@ -2398,15 +2643,19 @@
       <c r="D4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="34"/>
+      <c r="E4" s="46" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="81" t="s">
         <v>129</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -2429,12 +2678,16 @@
       <c r="E5" s="28">
         <v>1</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="96"/>
+      <c r="F5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="83">
+      <c r="I5" s="81">
         <v>1</v>
       </c>
       <c r="J5" s="17" t="s">
@@ -2451,18 +2704,22 @@
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="83" t="s">
+      <c r="I6" s="81" t="s">
         <v>134</v>
       </c>
       <c r="J6" s="17" t="s">
@@ -2479,18 +2736,22 @@
       <c r="C7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="96"/>
+      <c r="F7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="83" t="s">
+      <c r="I7" s="81" t="s">
         <v>137</v>
       </c>
       <c r="J7" s="17" t="s">
@@ -2507,18 +2768,22 @@
       <c r="C8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="96"/>
+      <c r="F8" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="81" t="s">
         <v>140</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -2535,18 +2800,22 @@
       <c r="C9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="96"/>
+      <c r="F9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="81" t="s">
         <v>143</v>
       </c>
       <c r="J9" s="17" t="s">
@@ -2566,15 +2835,19 @@
       <c r="D10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="103" t="s">
+      <c r="E10" s="96" t="s">
         <v>226</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="96"/>
+      <c r="F10" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="83">
+      <c r="I10" s="81">
         <v>10</v>
       </c>
       <c r="J10" s="17" t="s">
@@ -2591,18 +2864,22 @@
       <c r="C11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="96"/>
+      <c r="F11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="83" t="s">
+      <c r="I11" s="81" t="s">
         <v>149</v>
       </c>
       <c r="J11" s="17" t="s">
@@ -2619,18 +2896,22 @@
       <c r="C12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="96"/>
+        <v>248</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="83" t="s">
+      <c r="I12" s="81" t="s">
         <v>152</v>
       </c>
       <c r="J12" s="17" t="s">
@@ -2647,18 +2928,22 @@
       <c r="C13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="96"/>
+        <v>248</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="94" t="s">
+        <v>11</v>
+      </c>
       <c r="H13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="83" t="s">
+      <c r="I13" s="81" t="s">
         <v>155</v>
       </c>
       <c r="J13" s="17" t="s">
@@ -2678,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203F7812-755D-4EFC-B094-8BF895453DC0}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2714,7 +2999,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="78" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -2746,16 +3031,16 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="88" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="24" t="s">
@@ -2781,11 +3066,15 @@
       <c r="D4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="46" t="s">
         <v>228</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="85"/>
+      <c r="F4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="83" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
@@ -2809,11 +3098,15 @@
       <c r="D5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="93" t="s">
         <v>218</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="35"/>
+      <c r="F5" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H5" s="24" t="s">
         <v>11</v>
       </c>
@@ -2837,11 +3130,15 @@
       <c r="D6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="93" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="86"/>
-      <c r="G6" s="35"/>
+      <c r="F6" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
@@ -2865,11 +3162,15 @@
       <c r="D7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="95" t="s">
+      <c r="E7" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="F7" s="86"/>
-      <c r="G7" s="35"/>
+      <c r="F7" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
@@ -2896,8 +3197,12 @@
       <c r="E8" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="F8" s="86"/>
-      <c r="G8" s="35"/>
+      <c r="F8" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
@@ -2921,11 +3226,15 @@
       <c r="D9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="95" t="s">
+      <c r="E9" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="35"/>
+      <c r="F9" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H9" s="24" t="s">
         <v>11</v>
       </c>
@@ -2949,11 +3258,15 @@
       <c r="D10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="93" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="86"/>
-      <c r="G10" s="35"/>
+      <c r="F10" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H10" s="24" t="s">
         <v>11</v>
       </c>
@@ -2977,11 +3290,15 @@
       <c r="D11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="95" t="s">
+      <c r="E11" s="93" t="s">
         <v>216</v>
       </c>
-      <c r="F11" s="86"/>
-      <c r="G11" s="35"/>
+      <c r="F11" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
@@ -3008,8 +3325,12 @@
       <c r="E12" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="F12" s="86"/>
-      <c r="G12" s="35"/>
+      <c r="F12" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
@@ -3057,8 +3378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570AF19E-F26B-4187-B7FA-5CACB90F90DE}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3125,22 +3446,22 @@
       <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="94" t="s">
+      <c r="H3" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="83">
+      <c r="I3" s="81">
         <v>34658</v>
       </c>
       <c r="J3" s="17" t="s">
@@ -3161,18 +3482,18 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="94" t="s">
+      <c r="H4" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="81" t="s">
         <v>182</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -3195,16 +3516,16 @@
       <c r="E5" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="94" t="s">
+      <c r="H5" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="86" t="s">
+      <c r="I5" s="84" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="17" t="s">
@@ -3227,16 +3548,16 @@
       <c r="E6" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="94" t="s">
+      <c r="H6" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="86" t="s">
+      <c r="I6" s="84" t="s">
         <v>11</v>
       </c>
       <c r="J6" s="17" t="s">
@@ -3253,22 +3574,22 @@
       <c r="C7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="86" t="s">
+      <c r="E7" s="84" t="s">
         <v>187</v>
       </c>
-      <c r="F7" s="86" t="s">
+      <c r="F7" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="94" t="s">
+      <c r="H7" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="83" t="s">
+      <c r="I7" s="81" t="s">
         <v>187</v>
       </c>
       <c r="J7" s="17" t="s">
@@ -3291,16 +3612,16 @@
       <c r="E8" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="94" t="s">
+      <c r="H8" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="81" t="s">
         <v>190</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -3320,19 +3641,19 @@
       <c r="D9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="86" t="s">
-        <v>213</v>
-      </c>
-      <c r="F9" s="86" t="s">
+      <c r="E9" s="84" t="s">
+        <v>325</v>
+      </c>
+      <c r="F9" s="84" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="94" t="s">
+      <c r="H9" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="83">
+      <c r="I9" s="81">
         <v>17839</v>
       </c>
       <c r="J9" s="17" t="s">
@@ -3353,7 +3674,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>11</v>
@@ -3361,10 +3682,10 @@
       <c r="G10" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="94" t="s">
+      <c r="H10" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="83" t="s">
+      <c r="I10" s="81" t="s">
         <v>108</v>
       </c>
       <c r="J10" s="17" t="s">
@@ -3395,17 +3716,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E3782C-18A9-45D3-B018-D5B7F7291E9F}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="34.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="18.109375" style="2" customWidth="1"/>
@@ -3457,13 +3778,13 @@
       <c r="A3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="60" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="19" t="s">
@@ -3475,13 +3796,13 @@
       <c r="G3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="94" t="s">
+      <c r="H3" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="71" t="s">
+      <c r="J3" s="69" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3499,21 +3820,21 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="94" t="s">
+      <c r="H4" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="1:12" s="36" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
@@ -3526,28 +3847,28 @@
         <v>29</v>
       </c>
       <c r="D5" s="18"/>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="104" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="100" t="s">
+      <c r="G5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="94" t="s">
+      <c r="H5" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-    </row>
-    <row r="6" spans="1:12" s="36" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+    </row>
+    <row r="6" spans="1:12" s="36" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>66</v>
       </c>
@@ -3558,26 +3879,26 @@
         <v>29</v>
       </c>
       <c r="D6" s="18"/>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="100" t="s">
+      <c r="G6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="94" t="s">
+      <c r="H6" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="76" t="s">
+      <c r="I6" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="J6" s="40" t="s">
+      <c r="J6" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
@@ -3590,26 +3911,26 @@
         <v>11</v>
       </c>
       <c r="D7" s="18"/>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="98" t="s">
+      <c r="G7" s="105" t="s">
         <v>239</v>
       </c>
-      <c r="H7" s="94" t="s">
+      <c r="H7" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="72" t="s">
+      <c r="I7" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
     </row>
     <row r="8" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
@@ -3622,26 +3943,26 @@
         <v>11</v>
       </c>
       <c r="D8" s="18"/>
-      <c r="E8" s="99" t="s">
-        <v>212</v>
-      </c>
-      <c r="F8" s="97" t="s">
+      <c r="E8" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="100" t="s">
+      <c r="G8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="94" t="s">
+      <c r="H8" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="72">
+      <c r="I8" s="70">
         <v>48001</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
     </row>
     <row r="9" spans="1:12" s="36" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
@@ -3654,26 +3975,26 @@
         <v>29</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="100" t="s">
+      <c r="G9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="94" t="s">
+      <c r="H9" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="94" t="s">
+      <c r="I9" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
     </row>
     <row r="10" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
@@ -3686,26 +4007,26 @@
         <v>11</v>
       </c>
       <c r="D10" s="18"/>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="97" t="s">
+      <c r="F10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="100" t="s">
+      <c r="G10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="94" t="s">
+      <c r="H10" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="72" t="s">
+      <c r="I10" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
     </row>
     <row r="11" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
@@ -3718,26 +4039,26 @@
         <v>29</v>
       </c>
       <c r="D11" s="18"/>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="97" t="s">
+      <c r="F11" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="100" t="s">
+      <c r="G11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="94" t="s">
+      <c r="H11" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="75" t="s">
+      <c r="I11" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
     </row>
     <row r="12" spans="1:12" s="36" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
@@ -3750,89 +4071,89 @@
         <v>11</v>
       </c>
       <c r="D12" s="18"/>
-      <c r="E12" s="97" t="s">
+      <c r="E12" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="F12" s="97" t="s">
+      <c r="F12" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="100" t="s">
+      <c r="G12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="94" t="s">
+      <c r="H12" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="72" t="s">
+      <c r="I12" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="J12" s="40" t="s">
+      <c r="J12" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J13" s="45"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J14" s="45"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J15" s="45"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J16" s="45"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="23"/>
       <c r="D20" s="2"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="23"/>
       <c r="D21" s="2"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="23"/>
       <c r="D22" s="2"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="23"/>
       <c r="D23" s="2"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="23"/>
@@ -3867,8 +4188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E07544-54C6-4298-B1F4-AA27E9BE2694}">
   <dimension ref="A1:K16431"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:E12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3887,32 +4208,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="55" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -3926,16 +4247,16 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="59" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="14"/>
@@ -3947,21 +4268,21 @@
       <c r="I3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="48" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="60" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="19"/>
@@ -3973,21 +4294,21 @@
       <c r="I4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="50" t="s">
+      <c r="J4" s="48" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="60" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="19"/>
@@ -3999,21 +4320,21 @@
       <c r="I5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="48" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="60" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="19"/>
@@ -4025,21 +4346,21 @@
       <c r="I6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="48" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="60" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="19"/>
@@ -4051,21 +4372,21 @@
       <c r="I7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="48" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="60" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="19"/>
@@ -4077,28 +4398,28 @@
       <c r="I8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="48" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="110" t="s">
+      <c r="E9" s="103" t="s">
         <v>221</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="39"/>
+      <c r="F9" s="106"/>
+      <c r="G9" s="105"/>
       <c r="H9" s="16" t="s">
         <v>11</v>
       </c>
@@ -4111,22 +4432,22 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="109" t="s">
+      <c r="E10" s="102" t="s">
         <v>228</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="107"/>
       <c r="G10" s="22"/>
       <c r="H10" s="16" t="s">
         <v>11</v>
@@ -4140,22 +4461,23 @@
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="60" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="105"/>
       <c r="H11" s="16" t="s">
         <v>11</v>
       </c>
@@ -4167,23 +4489,23 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="60" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="39"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="105"/>
       <c r="H12" s="16" t="s">
         <v>11</v>
       </c>
@@ -4196,23 +4518,23 @@
       <c r="K12" s="36"/>
     </row>
     <row r="13" spans="1:11" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="48"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="110"/>
       <c r="H13" s="16" t="s">
         <v>11</v>
       </c>
@@ -4236,13 +4558,13 @@
       <c r="D14" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="16" t="s">
@@ -4251,7 +4573,7 @@
       <c r="I14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="50"/>
+      <c r="J14" s="48"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4266,14 +4588,14 @@
       <c r="D15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="111" t="s">
         <v>243</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="49" t="s">
-        <v>244</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>11</v>
@@ -4281,7 +4603,7 @@
       <c r="I15" s="27">
         <v>125483.1563</v>
       </c>
-      <c r="J15" s="50" t="s">
+      <c r="J15" s="48" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4298,20 +4620,20 @@
       <c r="D16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="25" t="s">
-        <v>245</v>
+      <c r="G16" s="35" t="s">
+        <v>244</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="J16" s="50" t="s">
+      <c r="J16" s="48" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4328,13 +4650,13 @@
       <c r="D17" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="16" t="s">
@@ -4343,7 +4665,7 @@
       <c r="I17" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="50" t="s">
+      <c r="J17" s="48" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4357,16 +4679,16 @@
       <c r="C18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="16" t="s">
@@ -4375,7 +4697,7 @@
       <c r="I18" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="48" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4389,16 +4711,16 @@
       <c r="C19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="16" t="s">
@@ -4407,7 +4729,7 @@
       <c r="I19" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J19" s="50" t="s">
+      <c r="J19" s="48" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4421,16 +4743,16 @@
       <c r="C20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="102">
-        <v>44106</v>
-      </c>
-      <c r="F20" s="24" t="s">
+      <c r="E20" s="112">
+        <v>44246</v>
+      </c>
+      <c r="F20" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="16" t="s">
@@ -4439,7 +4761,7 @@
       <c r="I20" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="J20" s="50" t="s">
+      <c r="J20" s="48" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4453,16 +4775,16 @@
       <c r="C21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="G21" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="16" t="s">
@@ -4471,7 +4793,7 @@
       <c r="I21" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="50" t="s">
+      <c r="J21" s="48" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4488,13 +4810,13 @@
       <c r="D22" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="16" t="s">
@@ -4503,7 +4825,7 @@
       <c r="I22" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="50" t="s">
+      <c r="J22" s="48" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4520,13 +4842,13 @@
       <c r="D23" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="16" t="s">
@@ -4535,7 +4857,7 @@
       <c r="I23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="48" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4552,13 +4874,13 @@
       <c r="D24" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="16" t="s">
@@ -4567,7 +4889,7 @@
       <c r="I24" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="50" t="s">
+      <c r="J24" s="48" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4581,16 +4903,16 @@
       <c r="C25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="16" t="s">
@@ -4599,7 +4921,7 @@
       <c r="I25" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="50" t="s">
+      <c r="J25" s="48" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4616,13 +4938,13 @@
       <c r="D26" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="16" t="s">
@@ -4631,7 +4953,7 @@
       <c r="I26" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="48" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4648,13 +4970,13 @@
       <c r="D27" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="25" t="s">
+      <c r="G27" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="16" t="s">
@@ -4663,7 +4985,7 @@
       <c r="I27" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="48" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4677,16 +4999,16 @@
       <c r="C28" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="F28" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="16" t="s">
@@ -4695,7 +5017,7 @@
       <c r="I28" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J28" s="50"/>
+      <c r="J28" s="48"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -4707,16 +5029,16 @@
       <c r="C29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="F29" s="24" t="s">
+      <c r="E29" s="84" t="s">
+        <v>199</v>
+      </c>
+      <c r="F29" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="25" t="s">
+      <c r="G29" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H29" s="16" t="s">
@@ -4725,7 +5047,7 @@
       <c r="I29" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="J29" s="50" t="s">
+      <c r="J29" s="48" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4739,17 +5061,17 @@
       <c r="C30" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="25" t="s">
-        <v>134</v>
+      <c r="G30" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>11</v>
@@ -4757,7 +5079,7 @@
       <c r="I30" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="J30" s="50" t="s">
+      <c r="J30" s="48" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4771,16 +5093,16 @@
       <c r="C31" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="G31" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="16" t="s">
@@ -4789,7 +5111,7 @@
       <c r="I31" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J31" s="50" t="s">
+      <c r="J31" s="48" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4803,17 +5125,17 @@
       <c r="C32" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="49" t="s">
+      <c r="D32" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="F32" s="24" t="s">
+      <c r="E32" s="84" t="s">
+        <v>329</v>
+      </c>
+      <c r="F32" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="25" t="s">
-        <v>11</v>
+      <c r="G32" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>11</v>
@@ -4821,7 +5143,7 @@
       <c r="I32" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="J32" s="50" t="s">
+      <c r="J32" s="48" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4835,17 +5157,17 @@
       <c r="C33" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="49" t="s">
+      <c r="D33" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="F33" s="24" t="s">
+      <c r="E33" s="84" t="s">
+        <v>328</v>
+      </c>
+      <c r="F33" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="25" t="s">
-        <v>11</v>
+      <c r="G33" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>11</v>
@@ -4853,25 +5175,25 @@
       <c r="I33" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="J33" s="50" t="s">
+      <c r="J33" s="48" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I34" s="27"/>
-      <c r="J34" s="50"/>
+      <c r="J34" s="48"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I35" s="27"/>
-      <c r="J35" s="50"/>
+      <c r="J35" s="48"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I36" s="27"/>
-      <c r="J36" s="50"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I37" s="27"/>
-      <c r="J37" s="50"/>
+      <c r="J37" s="48"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I38" s="27"/>
@@ -4903,7 +5225,7 @@
     <row r="51" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51" s="2"/>
-      <c r="D51" s="46"/>
+      <c r="D51" s="45"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52"/>
@@ -4951,12 +5273,12 @@
     <row r="66" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66" s="2"/>
-      <c r="D66" s="46"/>
+      <c r="D66" s="45"/>
     </row>
     <row r="67" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67" s="2"/>
-      <c r="D67" s="46"/>
+      <c r="D67" s="45"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68"/>
@@ -54078,4 +54400,395 @@
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7AACA6-44BD-46B9-9977-04909E4A448D}">
+  <dimension ref="A1:A74"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7500">
+    <sortCondition ref="A2:A7500"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>